<commit_message>
Insert row above top one.
</commit_message>
<xml_diff>
--- a/example/prototype.xlsx
+++ b/example/prototype.xlsx
@@ -194,6 +194,11 @@
   <borders count="53">
     <border/>
     <border>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
@@ -267,11 +272,6 @@
       <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-    </border>
-    <border>
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
@@ -649,29 +649,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -685,7 +686,7 @@
     <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="19" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="20" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="21" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -706,7 +707,7 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="30" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="31" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -716,7 +717,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="34" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -747,7 +748,7 @@
     <xf borderId="45" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="48" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -992,359 +993,377 @@
     <col customWidth="1" min="12" max="12" width="5.43"/>
   </cols>
   <sheetData>
-    <row r="1" ht="47.25" customHeight="1"/>
-    <row r="2" ht="50.25" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+    <row r="1" ht="17.25" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" ht="47.25" customHeight="1"/>
+    <row r="3" ht="50.25" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" ht="21.0" customHeight="1">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" ht="21.0" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15">
         <v>44179.0</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17" t="s">
+      <c r="H5" s="17"/>
+      <c r="I5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="19"/>
-    </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="22"/>
-    </row>
-    <row r="6" ht="20.25" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="9"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="20"/>
+    </row>
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
       <c r="K6" s="23"/>
     </row>
-    <row r="7" ht="21.0" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25" t="s">
+    <row r="7" ht="20.25" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="11"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" ht="21.0" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G8" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="29" t="s">
+      <c r="H8" s="28"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="30"/>
-    </row>
-    <row r="8" ht="21.75" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="30"/>
+      <c r="K8" s="31"/>
     </row>
     <row r="9" ht="21.75" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="32" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" ht="21.75" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="34" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="30"/>
-    </row>
-    <row r="10" ht="21.75" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="36" t="s">
+      <c r="J10" s="36"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" ht="21.75" customHeight="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="37">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="38">
         <v>2.5</v>
       </c>
-      <c r="J10" s="38"/>
-      <c r="K10" s="30"/>
-    </row>
-    <row r="11" ht="21.75" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="39"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="30"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" ht="21.75" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="43" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="40"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="31"/>
+    </row>
+    <row r="13" ht="21.75" customHeight="1">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="44"/>
-    </row>
-    <row r="13" ht="24.0" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="47"/>
-    </row>
-    <row r="14" ht="20.25" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="50"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="52" t="s">
+      <c r="J13" s="19"/>
+      <c r="K13" s="45"/>
+    </row>
+    <row r="14" ht="24.0" customHeight="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="48"/>
+    </row>
+    <row r="15" ht="20.25" customHeight="1">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="51"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="53"/>
-      <c r="H15" s="54" t="s">
+      <c r="G16" s="54"/>
+      <c r="H16" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="55" t="s">
+      <c r="I16" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="53"/>
-      <c r="K15" s="56"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="57" t="s">
+      <c r="J16" s="54"/>
+      <c r="K16" s="57"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="58"/>
-      <c r="H16" s="54" t="s">
+      <c r="G17" s="59"/>
+      <c r="H17" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="59"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="56"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="56"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="57"/>
     </row>
     <row r="18">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="60" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="57"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="58"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="56"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="56"/>
-    </row>
-    <row r="20" ht="21.75" customHeight="1">
-      <c r="A20" s="61"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="63" t="s">
+      <c r="H19" s="59"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="57"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="57"/>
+    </row>
+    <row r="21" ht="21.75" customHeight="1">
+      <c r="A21" s="62"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="64" t="s">
+      <c r="G21" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="64" t="s">
+      <c r="H21" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="65" t="s">
+      <c r="I21" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="58"/>
-      <c r="K20" s="66"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-    </row>
-    <row r="22" ht="53.25" customHeight="1"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="67"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" ht="53.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:K5"/>
+  <mergeCells count="46">
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:K6"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="E7:K7"/>
     <mergeCell ref="A8:D8"/>
-    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="E13:K13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:K14"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="E21:K21"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L2:O21"/>
-    <mergeCell ref="A22:O22"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="F9:J9"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="F10:H10"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="E14:K14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="E15:K15"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="E22:K22"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="L3:O22"/>
+    <mergeCell ref="A23:O23"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="A14:D14"/>
     <mergeCell ref="A16:D16"/>
-    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="I16:I17"/>
     <mergeCell ref="A17:D17"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="A18:D18"/>
-    <mergeCell ref="G18:H18"/>
     <mergeCell ref="A19:D19"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="A20:D20"/>
-    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="I21:J21"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>